<commit_message>
To be frank, I need to branch this off because it's been 48 days since a commit. New branch first mission is to update MCAO for all the columns we need for the dialer. Then we'll push back here and make sure all is well for the Batchdata testing & finally the build of the dialer.
</commit_message>
<xml_diff>
--- a/MCAO/MAX_HEADERS.xlsx
+++ b/MCAO/MAX_HEADERS.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/MCAO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45BFE9F-F0F8-7C40-9C35-721C9936DADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDF5BC7-4600-FB4B-AF1F-61FDDF8543C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="3700" windowWidth="26840" windowHeight="15940" xr2:uid="{79CD12A3-156F-714F-B30C-42F18A8FDF5D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{79CD12A3-156F-714F-B30C-42F18A8FDF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="MaxHeaders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>COUNTY</t>
   </si>
@@ -288,13 +288,79 @@
   </si>
   <si>
     <t>FULL_ADDRESS</t>
+  </si>
+  <si>
+    <t>IsRental</t>
+  </si>
+  <si>
+    <t>LocalJusidiction</t>
+  </si>
+  <si>
+    <t>MCR</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_0_UpdateDate</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_0_Url</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_1_UpdateDate</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_1_Url</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_2_UpdateDate</t>
+  </si>
+  <si>
+    <t>MapIDs_Book/Map Maps_2_Url</t>
+  </si>
+  <si>
+    <t>NumberOfParcelsInMCR</t>
+  </si>
+  <si>
+    <t>NumberOfParcelsInSTR</t>
+  </si>
+  <si>
+    <t>NumberOfParcelsInSubdivision</t>
+  </si>
+  <si>
+    <t>Owner_DeedType</t>
+  </si>
+  <si>
+    <t>Owner_SaleDate</t>
+  </si>
+  <si>
+    <t>PEPropUseDesc</t>
+  </si>
+  <si>
+    <t>PropertyAddress</t>
+  </si>
+  <si>
+    <t>PropertyDescription</t>
+  </si>
+  <si>
+    <t>ResidentialPropertyData_ConstructionYear</t>
+  </si>
+  <si>
+    <t>ResidentialPropertyData_ExteriorWalls</t>
+  </si>
+  <si>
+    <t>ResidentialPropertyData_ImprovementQualityGrade</t>
+  </si>
+  <si>
+    <t>Valuations_0_AssessedLPV</t>
+  </si>
+  <si>
+    <t>Valuations_0_AssessmentRatioPercentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,18 +369,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -344,10 +427,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,34 +463,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -651,15 +737,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8455E0F9-81AB-FC4B-9665-2640AD935615}">
-  <dimension ref="A1:CF1"/>
+  <dimension ref="A1:DB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:DB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:106" ht="96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -911,6 +997,72 @@
       </c>
       <c r="CF1" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="CG1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>